<commit_message>
Update 数据连接改为ALi - Druid
</commit_message>
<xml_diff>
--- a/src/main/resources/caseFiles/User.xlsx
+++ b/src/main/resources/caseFiles/User.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wecashtester/Desktop/GitFile/dubbo-interface/src/main/resources/caseFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6D4871-9B90-2746-8960-FB7AC628BF5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18630205-44DC-514A-9E6B-26DCE469F1C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getUser" sheetId="12" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>addr</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,10 +168,6 @@
   </si>
   <si>
     <t>jsonObjectParam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>errorParam</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -238,6 +234,22 @@
 "id":2,
 "age":80
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expectSQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM people WHERE id = 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM people WHERE id = 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -791,7 +803,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -810,7 +822,7 @@
     <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.6640625" customWidth="1"/>
     <col min="14" max="14" width="31" customWidth="1"/>
-    <col min="15" max="15" width="24.6640625" customWidth="1"/>
+    <col min="15" max="15" width="33.5" customWidth="1"/>
     <col min="16" max="16" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -855,93 +867,97 @@
         <v>13</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="114">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="M2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="P2" s="8"/>
     </row>
     <row r="3" spans="1:16" ht="114">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="N3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="P3" s="8"/>
     </row>
   </sheetData>

</xml_diff>